<commit_message>
Add new sample page where its markdown is read in from a markdown file
</commit_message>
<xml_diff>
--- a/data/test_page_metadata.xlsx
+++ b/data/test_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\Portfolio Website\portfolio-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3CCA92-4A6C-44A0-B5A9-3BEE792E6C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B27856D-3E9C-4C17-95C0-32BA11545F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>home</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>concepts</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>Sample</t>
   </si>
 </sst>
 </file>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2C412C-6E97-4788-869B-F51667F527C3}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -696,6 +702,26 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{CD681E0B-A6D3-4F29-93A0-129E2D09B503}"/>

</xml_diff>

<commit_message>
Add a real project page from the UCSD bootcamp
</commit_message>
<xml_diff>
--- a/data/test_page_metadata.xlsx
+++ b/data/test_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\Portfolio Website\portfolio-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B27856D-3E9C-4C17-95C0-32BA11545F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0C93C8-D577-4FD6-8425-3F1186CF3AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>home</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>Sample</t>
+  </si>
+  <si>
+    <t>credit_supervised</t>
+  </si>
+  <si>
+    <t>Credit Risk</t>
+  </si>
+  <si>
+    <t>pandas, sklearn, imblearn</t>
+  </si>
+  <si>
+    <t>resampling: oversampling, undersampling, combination sampling ensemble methods: random forest, AdaBoost</t>
   </si>
 </sst>
 </file>
@@ -523,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2C412C-6E97-4788-869B-F51667F527C3}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -722,14 +734,44 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="1:10" ht="34.799999999999997" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{CD681E0B-A6D3-4F29-93A0-129E2D09B503}"/>
     <hyperlink ref="F4" r:id="rId2" xr:uid="{2D920DAB-EFA3-435C-B571-C96879D2C73D}"/>
     <hyperlink ref="F5" r:id="rId3" xr:uid="{9D280C85-D79B-4336-9A15-038EBEDAD179}"/>
     <hyperlink ref="F6" r:id="rId4" xr:uid="{7AC7EFFB-3B11-487B-97D8-C67A867BDDF6}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{1C478062-D000-46F1-85F8-12FFBC2B4F50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove the dashboard page row from the metadata excel sheet
</commit_message>
<xml_diff>
--- a/data/test_page_metadata.xlsx
+++ b/data/test_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\Portfolio Website\portfolio-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6585FAD4-08FD-4F29-8EC4-C24DD5B18C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE7729D-05B3-4337-B390-74B4D6AB8BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>home</t>
   </si>
@@ -51,12 +51,6 @@
     <t>pandas, httpx, selectolax</t>
   </si>
   <si>
-    <t>pandas, splinter, selectolax, spacy</t>
-  </si>
-  <si>
-    <t>webs craping, OOP, NLP</t>
-  </si>
-  <si>
     <t>web scraping</t>
   </si>
   <si>
@@ -78,18 +72,12 @@
     <t>website</t>
   </si>
   <si>
-    <t>javascript</t>
-  </si>
-  <si>
     <t>https://github.com/cdpeters/handbell-music-validation</t>
   </si>
   <si>
     <t>https://github.com/cdpeters/mlb-the-show-analysis</t>
   </si>
   <si>
-    <t>https://github.com/cdpeters/crypto-clustering-unsupervised-ML-sklearn</t>
-  </si>
-  <si>
     <t>https://github.com/cdpeters/credit-risk-supervised-ML-sklearn</t>
   </si>
   <si>
@@ -108,12 +96,6 @@
     <t>background</t>
   </si>
   <si>
-    <t>dashboard</t>
-  </si>
-  <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
     <t>sidebar</t>
   </si>
   <si>
@@ -145,6 +127,9 @@
   </si>
   <si>
     <t xml:space="preserve">pandas, splinter, bs4 (beautiful soup 4), sqlalchemy, bootstrap, AWS, postgresql, flask </t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -202,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -215,6 +200,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -535,16 +523,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2C412C-6E97-4788-869B-F51667F527C3}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" style="9" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -558,42 +546,42 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="b">
-        <v>1</v>
+      <c r="B2" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
@@ -606,10 +594,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1" t="b">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -618,10 +606,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>3</v>
@@ -631,8 +619,8 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="b">
-        <v>1</v>
+      <c r="B4" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="C4" s="7">
         <v>2</v>
@@ -641,10 +629,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>6</v>
@@ -653,125 +641,95 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="1" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="C5" s="7">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="b">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="C6" s="7">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
+        <v>27</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="7">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{CD681E0B-A6D3-4F29-93A0-129E2D09B503}"/>
     <hyperlink ref="F4" r:id="rId2" xr:uid="{2D920DAB-EFA3-435C-B571-C96879D2C73D}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{9D280C85-D79B-4336-9A15-038EBEDAD179}"/>
-    <hyperlink ref="F6" r:id="rId4" xr:uid="{7AC7EFFB-3B11-487B-97D8-C67A867BDDF6}"/>
-    <hyperlink ref="F8" r:id="rId5" xr:uid="{1C478062-D000-46F1-85F8-12FFBC2B4F50}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{7AC7EFFB-3B11-487B-97D8-C67A867BDDF6}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{1C478062-D000-46F1-85F8-12FFBC2B4F50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>